<commit_message>
-- Update providers email
</commit_message>
<xml_diff>
--- a/storage/macros/cuarto/Datos de salida.xlsx
+++ b/storage/macros/cuarto/Datos de salida.xlsx
@@ -150,38 +150,38 @@
       <sheetData sheetId="2">
         <row r="5">
           <cell r="K5" t="str">
-            <v>BHA850</v>
+            <v>BMA600</v>
           </cell>
           <cell r="L5">
-            <v>85000</v>
+            <v>60000</v>
           </cell>
           <cell r="P5">
-            <v>35728000</v>
+            <v>14442000</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="5">
           <cell r="L5" t="str">
-            <v>BD0751H2</v>
+            <v>BD0501M6</v>
           </cell>
           <cell r="M5">
-            <v>96300</v>
+            <v>56740</v>
           </cell>
           <cell r="Q5">
-            <v>13920000</v>
+            <v>22040000</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
         <row r="3">
           <cell r="D3">
-            <v>512.5</v>
+            <v>320</v>
           </cell>
         </row>
         <row r="4">
           <cell r="H4">
-            <v>30000</v>
+            <v>20000</v>
           </cell>
         </row>
         <row r="5">
@@ -191,7 +191,7 @@
         </row>
         <row r="7">
           <cell r="D7">
-            <v>749</v>
+            <v>550</v>
           </cell>
         </row>
         <row r="14">
@@ -223,7 +223,7 @@
         </row>
         <row r="10">
           <cell r="D10">
-            <v>8</v>
+            <v>48</v>
           </cell>
         </row>
         <row r="14">
@@ -243,7 +243,7 @@
         </row>
         <row r="17">
           <cell r="D17">
-            <v>4</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="20">
@@ -263,7 +263,7 @@
         </row>
         <row r="23">
           <cell r="C23">
-            <v>104</v>
+            <v>516</v>
           </cell>
         </row>
         <row r="24">
@@ -624,18 +624,18 @@
       </c>
       <c r="B2" t="str">
         <f>[1]Evaporadoras!$K$5</f>
-        <v>BHA850</v>
+        <v>BMA600</v>
       </c>
       <c r="C2">
         <f>[1]Evaporadoras!$L$5</f>
-        <v>85000</v>
+        <v>60000</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>[1]Evaporadoras!$P$5</f>
-        <v>35728000</v>
+        <v>14442000</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -647,18 +647,18 @@
       </c>
       <c r="B3" t="str">
         <f>[1]Condensadoras!$L$5</f>
-        <v>BD0751H2</v>
+        <v>BD0501M6</v>
       </c>
       <c r="C3">
         <f>[1]Condensadoras!$M$5</f>
-        <v>96300</v>
+        <v>56740</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
         <f>[1]Condensadoras!$Q$5</f>
-        <v>13920000</v>
+        <v>22040000</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -673,15 +673,15 @@
       </c>
       <c r="E4">
         <f>[1]Soportes!$H$4</f>
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F4">
         <f>[1]Soportes!$D$3</f>
-        <v>512.5</v>
+        <v>320</v>
       </c>
       <c r="G4">
         <f>[1]Soportes!$D$7</f>
-        <v>749</v>
+        <v>550</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="D6">
         <f>[1]Estantes!$D$10</f>
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <f>[1]Estantes!$C$27</f>
@@ -744,7 +744,7 @@
       </c>
       <c r="D7">
         <f>[1]Estantes!$D$17</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <f>[1]Estantes!$C$28</f>
@@ -772,7 +772,7 @@
       </c>
       <c r="D8">
         <f>[1]Estantes!$C$23</f>
-        <v>104</v>
+        <v>516</v>
       </c>
       <c r="E8">
         <f>[1]Estantes!$C$24</f>
@@ -817,7 +817,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Complete cold room process
</commit_message>
<xml_diff>
--- a/storage/macros/cuarto/Datos de salida.xlsx
+++ b/storage/macros/cuarto/Datos de salida.xlsx
@@ -150,13 +150,13 @@
       <sheetData sheetId="2">
         <row r="5">
           <cell r="K5" t="str">
-            <v>BMA600</v>
+            <v>BHG 450</v>
           </cell>
           <cell r="L5">
-            <v>60000</v>
+            <v>49500</v>
           </cell>
           <cell r="P5">
-            <v>14442000</v>
+            <v>34655000</v>
           </cell>
         </row>
       </sheetData>
@@ -176,12 +176,12 @@
       <sheetData sheetId="4">
         <row r="3">
           <cell r="D3">
-            <v>320</v>
+            <v>512.5</v>
           </cell>
         </row>
         <row r="4">
           <cell r="H4">
-            <v>20000</v>
+            <v>30000</v>
           </cell>
         </row>
         <row r="5">
@@ -191,7 +191,7 @@
         </row>
         <row r="7">
           <cell r="D7">
-            <v>550</v>
+            <v>749</v>
           </cell>
         </row>
         <row r="14">
@@ -223,7 +223,7 @@
         </row>
         <row r="10">
           <cell r="D10">
-            <v>48</v>
+            <v>9</v>
           </cell>
         </row>
         <row r="14">
@@ -243,7 +243,7 @@
         </row>
         <row r="17">
           <cell r="D17">
-            <v>6</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="20">
@@ -263,7 +263,7 @@
         </row>
         <row r="23">
           <cell r="C23">
-            <v>516</v>
+            <v>108</v>
           </cell>
         </row>
         <row r="24">
@@ -624,18 +624,18 @@
       </c>
       <c r="B2" t="str">
         <f>[1]Evaporadoras!$K$5</f>
-        <v>BMA600</v>
+        <v>BHG 450</v>
       </c>
       <c r="C2">
         <f>[1]Evaporadoras!$L$5</f>
-        <v>60000</v>
+        <v>49500</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>[1]Evaporadoras!$P$5</f>
-        <v>14442000</v>
+        <v>34655000</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -673,15 +673,15 @@
       </c>
       <c r="E4">
         <f>[1]Soportes!$H$4</f>
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F4">
         <f>[1]Soportes!$D$3</f>
-        <v>320</v>
+        <v>512.5</v>
       </c>
       <c r="G4">
         <f>[1]Soportes!$D$7</f>
-        <v>550</v>
+        <v>749</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="D6">
         <f>[1]Estantes!$D$10</f>
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <f>[1]Estantes!$C$27</f>
@@ -744,7 +744,7 @@
       </c>
       <c r="D7">
         <f>[1]Estantes!$D$17</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f>[1]Estantes!$C$28</f>
@@ -772,7 +772,7 @@
       </c>
       <c r="D8">
         <f>[1]Estantes!$C$23</f>
-        <v>516</v>
+        <v>108</v>
       </c>
       <c r="E8">
         <f>[1]Estantes!$C$24</f>
@@ -817,7 +817,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>